<commit_message>
font sizes and skeleton loading
</commit_message>
<xml_diff>
--- a/frontend/public/assets/files/BIMei Macro Adoption Study.xlsx
+++ b/frontend/public/assets/files/BIMei Macro Adoption Study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MiguelProjects\02. Projects\7)Macro BIM adoption\frontend\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709C6AF5-A564-4F38-B9F0-561EDBD0D54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A201E7-E886-4404-BFCD-F25DF3959290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Questionnaire" sheetId="3" r:id="rId1"/>
@@ -2936,11 +2936,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3246,10 +3246,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF27FF1-CBF6-495C-A2ED-F8D7B692A940}">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A2:E60"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3259,11 +3259,6 @@
     <col min="4" max="4" width="46.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="9" t="s">
-        <v>925</v>
-      </c>
-    </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>913</v>
@@ -3314,7 +3309,7 @@
       <c r="C9" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>920</v>
       </c>
     </row>
@@ -3330,7 +3325,7 @@
       <c r="C11" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>920</v>
       </c>
     </row>
@@ -3338,7 +3333,7 @@
       <c r="C12" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>920</v>
       </c>
     </row>
@@ -3346,7 +3341,7 @@
       <c r="C13" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>924</v>
       </c>
     </row>
@@ -3495,7 +3490,7 @@
       <c r="C35" s="3"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="8" t="s">
         <v>921</v>
       </c>
       <c r="C36" s="3" t="s">
@@ -3509,7 +3504,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
+      <c r="A37" s="8"/>
       <c r="C37" s="3" t="s">
         <v>294</v>
       </c>
@@ -3521,7 +3516,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
+      <c r="A38" s="8"/>
       <c r="C38" s="3" t="s">
         <v>296</v>
       </c>
@@ -3533,7 +3528,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
+      <c r="A39" s="8"/>
       <c r="C39" s="3" t="s">
         <v>295</v>
       </c>
@@ -3542,18 +3537,18 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
+      <c r="A40" s="8"/>
       <c r="C40" s="3"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
+      <c r="A41" s="8"/>
       <c r="B41" s="4" t="s">
         <v>917</v>
       </c>
       <c r="C41" s="3"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
+      <c r="A42" s="8"/>
       <c r="C42" s="3" t="s">
         <v>281</v>
       </c>
@@ -3565,7 +3560,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
+      <c r="A43" s="8"/>
       <c r="C43" s="3" t="s">
         <v>289</v>
       </c>
@@ -3577,7 +3572,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
+      <c r="A44" s="8"/>
       <c r="C44" s="3" t="s">
         <v>282</v>
       </c>
@@ -3709,8 +3704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCF85EA6-125E-47DB-87D7-2082C385594A}">
   <dimension ref="B2:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3730,8 +3725,14 @@
         <v>928</v>
       </c>
     </row>
+    <row r="9" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="9" t="s">
+        <v>925</v>
+      </c>
+    </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
         <v>929</v>
       </c>
     </row>

</xml_diff>

<commit_message>
text center, xaxis domain limits, legend style
</commit_message>
<xml_diff>
--- a/frontend/public/assets/files/BIMei Macro Adoption Study.xlsx
+++ b/frontend/public/assets/files/BIMei Macro Adoption Study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MiguelProjects\02. Projects\7)Macro BIM adoption\frontend\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BAB57E-E303-46A9-923E-2A473CBFE9AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6297AF9-0E88-4F02-8AE3-627F8BC8CA98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Questionnaire" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28733" uniqueCount="931">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28736" uniqueCount="934">
   <si>
     <t>User ID</t>
   </si>
@@ -2820,6 +2820,15 @@
   <si>
     <t>consider the field others as a separate category!!</t>
   </si>
+  <si>
+    <t>redondearlo al más alto a cada 5</t>
+  </si>
+  <si>
+    <t>titulo centrado</t>
+  </si>
+  <si>
+    <t>others to None! In the last 3 charts</t>
+  </si>
 </sst>
 </file>
 
@@ -3251,8 +3260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF27FF1-CBF6-495C-A2ED-F8D7B692A940}">
   <dimension ref="A2:E60"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3705,10 +3714,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCF85EA6-125E-47DB-87D7-2082C385594A}">
-  <dimension ref="B2:B12"/>
+  <dimension ref="B2:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9:I10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3742,6 +3751,21 @@
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>930</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>933</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
preparing data to set the table component
</commit_message>
<xml_diff>
--- a/frontend/public/assets/files/BIMei Macro Adoption Study.xlsx
+++ b/frontend/public/assets/files/BIMei Macro Adoption Study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MiguelProjects\02. Projects\7)Macro BIM adoption\frontend\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6297AF9-0E88-4F02-8AE3-627F8BC8CA98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D46F328-379F-4C0F-9BDE-16051693047F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Questionnaire" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28736" uniqueCount="934">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28739" uniqueCount="938">
   <si>
     <t>User ID</t>
   </si>
@@ -2755,15 +2755,6 @@
     <t>No need to analyse</t>
   </si>
   <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>Graph</t>
-  </si>
-  <si>
-    <t>Text, let's discuss how to present this information</t>
-  </si>
-  <si>
     <t>All responses should merge into a single answer. One reality.</t>
   </si>
   <si>
@@ -2828,6 +2819,27 @@
   </si>
   <si>
     <t>others to None! In the last 3 charts</t>
+  </si>
+  <si>
+    <t>Pendientes</t>
+  </si>
+  <si>
+    <t>Text ajustar</t>
+  </si>
+  <si>
+    <t>Otros visualización</t>
+  </si>
+  <si>
+    <t>Horizontal</t>
+  </si>
+  <si>
+    <t>Horizontal (5)</t>
+  </si>
+  <si>
+    <t>Tabla</t>
+  </si>
+  <si>
+    <t>Table</t>
   </si>
 </sst>
 </file>
@@ -3260,8 +3272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF27FF1-CBF6-495C-A2ED-F8D7B692A940}">
   <dimension ref="A2:E60"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C33" sqref="C32:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3273,7 +3285,7 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3313,7 +3325,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
       <c r="C8" s="3"/>
     </row>
@@ -3322,7 +3334,7 @@
         <v>259</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3330,7 +3342,7 @@
         <v>266</v>
       </c>
       <c r="D10" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3338,7 +3350,7 @@
         <v>261</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3346,7 +3358,7 @@
         <v>262</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3354,7 +3366,7 @@
         <v>263</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3363,7 +3375,7 @@
         <v>264</v>
       </c>
       <c r="D14" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3372,7 +3384,7 @@
         <v>277</v>
       </c>
       <c r="D16" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3381,7 +3393,7 @@
         <v>260</v>
       </c>
       <c r="D17" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3390,7 +3402,7 @@
         <v>265</v>
       </c>
       <c r="D18" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3398,7 +3410,7 @@
         <v>268</v>
       </c>
       <c r="D19" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3409,7 +3421,7 @@
         <v>267</v>
       </c>
       <c r="D22" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3417,7 +3429,7 @@
         <v>269</v>
       </c>
       <c r="D23" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3425,7 +3437,7 @@
         <v>271</v>
       </c>
       <c r="D24" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3433,7 +3445,7 @@
         <v>272</v>
       </c>
       <c r="D25" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3441,18 +3453,18 @@
         <v>273</v>
       </c>
       <c r="D26" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>274</v>
       </c>
       <c r="D27" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3463,7 +3475,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
       <c r="C30" s="3"/>
     </row>
@@ -3472,7 +3484,7 @@
         <v>270</v>
       </c>
       <c r="D31" t="s">
-        <v>910</v>
+        <v>917</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3480,7 +3492,7 @@
         <v>279</v>
       </c>
       <c r="D32" t="s">
-        <v>910</v>
+        <v>935</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3489,7 +3501,7 @@
         <v>278</v>
       </c>
       <c r="D33" t="s">
-        <v>911</v>
+        <v>936</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -3497,22 +3509,22 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
       <c r="C35" s="3"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>280</v>
       </c>
       <c r="D36" t="s">
-        <v>910</v>
+        <v>917</v>
       </c>
       <c r="E36" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3521,10 +3533,10 @@
         <v>294</v>
       </c>
       <c r="D37" t="s">
-        <v>910</v>
+        <v>934</v>
       </c>
       <c r="E37" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3533,10 +3545,10 @@
         <v>296</v>
       </c>
       <c r="D38" t="s">
-        <v>910</v>
+        <v>935</v>
       </c>
       <c r="E38" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -3545,7 +3557,7 @@
         <v>295</v>
       </c>
       <c r="D39" t="s">
-        <v>909</v>
+        <v>936</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3555,7 +3567,7 @@
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="9"/>
       <c r="B41" s="4" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
       <c r="C41" s="3"/>
     </row>
@@ -3565,10 +3577,10 @@
         <v>281</v>
       </c>
       <c r="D42" t="s">
-        <v>910</v>
+        <v>917</v>
       </c>
       <c r="E42" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -3577,10 +3589,10 @@
         <v>289</v>
       </c>
       <c r="D43" t="s">
-        <v>910</v>
+        <v>934</v>
       </c>
       <c r="E43" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3589,10 +3601,10 @@
         <v>282</v>
       </c>
       <c r="D44" t="s">
+        <v>936</v>
+      </c>
+      <c r="E44" t="s">
         <v>909</v>
-      </c>
-      <c r="E44" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3600,7 +3612,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
       <c r="C46" s="3"/>
     </row>
@@ -3609,7 +3621,7 @@
         <v>283</v>
       </c>
       <c r="D47" t="s">
-        <v>910</v>
+        <v>917</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -3617,7 +3629,7 @@
         <v>285</v>
       </c>
       <c r="D48" t="s">
-        <v>910</v>
+        <v>935</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
@@ -3625,7 +3637,7 @@
         <v>286</v>
       </c>
       <c r="D49" t="s">
-        <v>910</v>
+        <v>935</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
@@ -3633,7 +3645,7 @@
         <v>287</v>
       </c>
       <c r="D50" t="s">
-        <v>910</v>
+        <v>917</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
@@ -3641,7 +3653,7 @@
         <v>288</v>
       </c>
       <c r="D51" t="s">
-        <v>911</v>
+        <v>937</v>
       </c>
     </row>
     <row r="52" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3649,7 +3661,7 @@
     </row>
     <row r="53" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="C53" s="3"/>
     </row>
@@ -3658,10 +3670,10 @@
         <v>290</v>
       </c>
       <c r="D54" t="s">
-        <v>910</v>
+        <v>917</v>
       </c>
       <c r="E54" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
@@ -3669,10 +3681,10 @@
         <v>284</v>
       </c>
       <c r="D55" t="s">
-        <v>910</v>
+        <v>935</v>
       </c>
       <c r="E55" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
@@ -3680,10 +3692,10 @@
         <v>291</v>
       </c>
       <c r="D56" t="s">
-        <v>910</v>
+        <v>935</v>
       </c>
       <c r="E56" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
@@ -3691,7 +3703,7 @@
         <v>292</v>
       </c>
       <c r="D57" t="s">
-        <v>911</v>
+        <v>937</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
@@ -3714,58 +3726,70 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCF85EA6-125E-47DB-87D7-2082C385594A}">
-  <dimension ref="B2:B20"/>
+  <dimension ref="B2:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="5" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="8" t="s">
+        <v>922</v>
+      </c>
+      <c r="H10" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
         <v>926</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>927</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
         <v>928</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="8" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>930</v>
-      </c>
-    </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
-        <v>931</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
     </row>
   </sheetData>
@@ -3777,8 +3801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O2684"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M2687" sqref="M2687"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
chart title text clamp to 3 lines max
</commit_message>
<xml_diff>
--- a/frontend/public/assets/files/BIMei Macro Adoption Study.xlsx
+++ b/frontend/public/assets/files/BIMei Macro Adoption Study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MiguelProjects\02. Projects\7)Macro BIM adoption\frontend\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D46F328-379F-4C0F-9BDE-16051693047F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A2F1E7-A138-442B-8CB5-3056A1FE1DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Questionnaire" sheetId="3" r:id="rId1"/>
@@ -2782,9 +2782,6 @@
     <t>Pie</t>
   </si>
   <si>
-    <t>desaparece</t>
-  </si>
-  <si>
     <t>+44 07401894416</t>
   </si>
   <si>
@@ -2840,6 +2837,9 @@
   </si>
   <si>
     <t>Table</t>
+  </si>
+  <si>
+    <t>desaparece o juntarlo como: ["Educational Framework"]</t>
   </si>
 </sst>
 </file>
@@ -2963,7 +2963,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3272,8 +3272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF27FF1-CBF6-495C-A2ED-F8D7B692A940}">
   <dimension ref="A2:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C33" sqref="C32:C33"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3342,7 +3342,7 @@
         <v>266</v>
       </c>
       <c r="D10" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3366,7 +3366,7 @@
         <v>263</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3375,7 +3375,7 @@
         <v>264</v>
       </c>
       <c r="D14" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3384,7 +3384,7 @@
         <v>277</v>
       </c>
       <c r="D16" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3393,7 +3393,7 @@
         <v>260</v>
       </c>
       <c r="D17" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3402,7 +3402,7 @@
         <v>265</v>
       </c>
       <c r="D18" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3410,7 +3410,7 @@
         <v>268</v>
       </c>
       <c r="D19" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3421,7 +3421,7 @@
         <v>267</v>
       </c>
       <c r="D22" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3429,7 +3429,7 @@
         <v>269</v>
       </c>
       <c r="D23" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3437,7 +3437,7 @@
         <v>271</v>
       </c>
       <c r="D24" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3445,7 +3445,7 @@
         <v>272</v>
       </c>
       <c r="D25" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3453,18 +3453,18 @@
         <v>273</v>
       </c>
       <c r="D26" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>274</v>
       </c>
       <c r="D27" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3492,7 +3492,7 @@
         <v>279</v>
       </c>
       <c r="D32" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3501,7 +3501,7 @@
         <v>278</v>
       </c>
       <c r="D33" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -3515,7 +3515,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>918</v>
+        <v>937</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>280</v>
@@ -3533,7 +3533,7 @@
         <v>294</v>
       </c>
       <c r="D37" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="E37" t="s">
         <v>909</v>
@@ -3545,7 +3545,7 @@
         <v>296</v>
       </c>
       <c r="D38" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="E38" t="s">
         <v>909</v>
@@ -3557,7 +3557,7 @@
         <v>295</v>
       </c>
       <c r="D39" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3589,7 +3589,7 @@
         <v>289</v>
       </c>
       <c r="D43" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="E43" t="s">
         <v>909</v>
@@ -3601,7 +3601,7 @@
         <v>282</v>
       </c>
       <c r="D44" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="E44" t="s">
         <v>909</v>
@@ -3629,7 +3629,7 @@
         <v>285</v>
       </c>
       <c r="D48" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
@@ -3637,7 +3637,7 @@
         <v>286</v>
       </c>
       <c r="D49" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
@@ -3653,7 +3653,7 @@
         <v>288</v>
       </c>
       <c r="D51" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="52" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3681,7 +3681,7 @@
         <v>284</v>
       </c>
       <c r="D55" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="E55" t="s">
         <v>909</v>
@@ -3692,7 +3692,7 @@
         <v>291</v>
       </c>
       <c r="D56" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="E56" t="s">
         <v>909</v>
@@ -3703,7 +3703,7 @@
         <v>292</v>
       </c>
       <c r="D57" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
@@ -3736,60 +3736,60 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H7" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H9" s="5" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="H10" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data stored in postgresql
</commit_message>
<xml_diff>
--- a/frontend/public/assets/files/BIMei Macro Adoption Study.xlsx
+++ b/frontend/public/assets/files/BIMei Macro Adoption Study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MiguelProjects\02. Projects\7)Macro BIM adoption\frontend\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C321D95-438D-45EB-9F82-F65D8195F88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733A5913-F0A3-45C4-98B0-35CA6B1BB574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Questionnaire" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Answers" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Answers!$H$1:$H$2684</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Answers!$G$1:$G$2684</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Questionnaire!$C$2:$C$60</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -3272,13 +3273,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF27FF1-CBF6-495C-A2ED-F8D7B692A940}">
   <dimension ref="A2:E60"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="111.28515625" customWidth="1"/>
     <col min="4" max="4" width="46.5703125" customWidth="1"/>
   </cols>
@@ -3289,6 +3291,9 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1696139171941</v>
+      </c>
       <c r="C3" s="3" t="s">
         <v>276</v>
       </c>
@@ -3297,6 +3302,9 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1696139477406</v>
+      </c>
       <c r="C4" s="3" t="s">
         <v>275</v>
       </c>
@@ -3305,6 +3313,9 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1696139949919</v>
+      </c>
       <c r="C5" s="3" t="s">
         <v>258</v>
       </c>
@@ -3313,6 +3324,9 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1696140883180</v>
+      </c>
       <c r="C6" s="3" t="s">
         <v>297</v>
       </c>
@@ -3321,7 +3335,12 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="3"/>
+      <c r="B7">
+        <v>1697541525184</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
@@ -3716,6 +3735,7 @@
       <c r="C60" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="C2:C60" xr:uid="{AFF27FF1-CBF6-495C-A2ED-F8D7B692A940}"/>
   <mergeCells count="1">
     <mergeCell ref="A36:A44"/>
   </mergeCells>
@@ -3802,8 +3822,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O2684"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2451" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A2686" sqref="A2686"/>
+    <sheetView topLeftCell="H1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3983,7 +4003,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -4572,8 +4592,8 @@
       <c r="F20" t="s">
         <v>217</v>
       </c>
-      <c r="G20" t="s">
-        <v>236</v>
+      <c r="G20">
+        <v>1696139171941</v>
       </c>
       <c r="H20" t="s">
         <v>276</v>
@@ -5199,7 +5219,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -5374,7 +5394,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="42" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>16</v>
       </c>
@@ -5406,7 +5426,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -7080,7 +7100,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>17</v>
       </c>
@@ -8100,7 +8120,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="121" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>17</v>
       </c>
@@ -8444,7 +8464,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>18</v>
       </c>
@@ -9354,7 +9374,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="157" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>18</v>
       </c>
@@ -9724,7 +9744,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="168" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>19</v>
       </c>
@@ -10036,7 +10056,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>19</v>
       </c>
@@ -11091,7 +11111,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="208" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>20</v>
       </c>
@@ -11931,7 +11951,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="232" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>20</v>
       </c>
@@ -12671,7 +12691,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="254" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>21</v>
       </c>
@@ -13535,7 +13555,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="281" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>21</v>
       </c>
@@ -13949,7 +13969,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="293" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>22</v>
       </c>
@@ -13981,7 +14001,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="294" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>22</v>
       </c>
@@ -15132,7 +15152,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="328" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>23</v>
       </c>
@@ -15762,7 +15782,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="346" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>23</v>
       </c>
@@ -16712,7 +16732,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="374" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>24</v>
       </c>
@@ -17129,7 +17149,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="386" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>24</v>
       </c>
@@ -17860,7 +17880,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="408" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>25</v>
       </c>
@@ -18490,7 +18510,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="426" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>25</v>
       </c>
@@ -19160,7 +19180,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="446" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>26</v>
       </c>
@@ -20210,7 +20230,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="476" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
         <v>26</v>
       </c>
@@ -20472,7 +20492,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="484" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
         <v>27</v>
       </c>
@@ -21728,7 +21748,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="521" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A521" t="s">
         <v>27</v>
       </c>
@@ -21757,7 +21777,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="522" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A522" t="s">
         <v>28</v>
       </c>
@@ -22034,7 +22054,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="530" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
         <v>28</v>
       </c>
@@ -23979,7 +23999,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="586" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="586" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A586" t="s">
         <v>29</v>
       </c>
@@ -24477,7 +24497,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="601" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="601" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A601" t="s">
         <v>29</v>
       </c>
@@ -24716,7 +24736,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="608" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="608" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A608" t="s">
         <v>30</v>
       </c>
@@ -24958,7 +24978,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="615" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="615" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A615" t="s">
         <v>30</v>
       </c>
@@ -26763,7 +26783,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="667" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="667" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A667" t="s">
         <v>31</v>
       </c>
@@ -27220,7 +27240,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="681" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="681" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A681" t="s">
         <v>31</v>
       </c>
@@ -27809,7 +27829,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="698" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="698" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A698" t="s">
         <v>32</v>
       </c>
@@ -28581,7 +28601,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="721" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="721" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A721" t="s">
         <v>32</v>
       </c>
@@ -28820,7 +28840,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="728" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="728" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A728" t="s">
         <v>33</v>
       </c>
@@ -29520,7 +29540,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="748" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="748" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A748" t="s">
         <v>33</v>
       </c>
@@ -30458,7 +30478,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="776" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="776" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A776" t="s">
         <v>34</v>
       </c>
@@ -30878,7 +30898,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="788" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="788" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A788" t="s">
         <v>34</v>
       </c>
@@ -31863,7 +31883,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="817" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="817" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A817" t="s">
         <v>35</v>
       </c>
@@ -32658,7 +32678,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="841" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="841" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A841" t="s">
         <v>35</v>
       </c>
@@ -32687,7 +32707,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="842" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="842" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A842" t="s">
         <v>36</v>
       </c>
@@ -32999,7 +33019,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="851" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="851" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A851" t="s">
         <v>36</v>
       </c>
@@ -34392,7 +34412,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="892" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="892" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A892" t="s">
         <v>37</v>
       </c>
@@ -35320,7 +35340,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="921" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="921" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A921" t="s">
         <v>37</v>
       </c>
@@ -35349,7 +35369,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="922" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="922" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A922" t="s">
         <v>38</v>
       </c>
@@ -35871,7 +35891,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="937" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="937" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A937" t="s">
         <v>38</v>
       </c>
@@ -36970,7 +36990,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="969" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="969" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A969" t="s">
         <v>39</v>
       </c>
@@ -38063,7 +38083,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1001" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1001" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1001" t="s">
         <v>39</v>
       </c>
@@ -38267,7 +38287,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1007" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1007" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1007" t="s">
         <v>40</v>
       </c>
@@ -39433,7 +39453,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="1041" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1041" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1041" t="s">
         <v>40</v>
       </c>
@@ -39777,7 +39797,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="1051" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1051" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1051" t="s">
         <v>41</v>
       </c>
@@ -40737,7 +40757,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1081" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1081" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1081" t="s">
         <v>41</v>
       </c>
@@ -41011,7 +41031,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="1089" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1089" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1089" t="s">
         <v>42</v>
       </c>
@@ -41291,7 +41311,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="1097" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1097" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1097" t="s">
         <v>42</v>
       </c>
@@ -42177,7 +42197,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="1123" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1123" t="s">
         <v>43</v>
       </c>
@@ -42419,7 +42439,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="1130" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1130" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1130" t="s">
         <v>43</v>
       </c>
@@ -44241,7 +44261,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1183" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1183" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1183" t="s">
         <v>44</v>
       </c>
@@ -44838,7 +44858,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1201" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1201" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1201" t="s">
         <v>44</v>
       </c>
@@ -44972,7 +44992,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1205" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1205" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1205" t="s">
         <v>45</v>
       </c>
@@ -46202,7 +46222,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1241" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1241" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1241" t="s">
         <v>45</v>
       </c>
@@ -46649,7 +46669,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="1253" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1253" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1253" t="s">
         <v>46</v>
       </c>
@@ -47698,7 +47718,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="1281" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1281" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1281" t="s">
         <v>46</v>
       </c>
@@ -48290,7 +48310,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1298" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1298" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1298" t="s">
         <v>47</v>
       </c>
@@ -49050,7 +49070,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1321" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1321" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1321" t="s">
         <v>47</v>
       </c>
@@ -49149,7 +49169,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1324" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1324" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1324" t="s">
         <v>48</v>
       </c>
@@ -50414,7 +50434,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1361" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1361" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1361" t="s">
         <v>48</v>
       </c>
@@ -50933,7 +50953,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="1376" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1376" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1376" t="s">
         <v>49</v>
       </c>
@@ -51733,7 +51753,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1401" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1401" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1401" t="s">
         <v>49</v>
       </c>
@@ -51937,7 +51957,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1407" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1407" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1407" t="s">
         <v>50</v>
       </c>
@@ -52147,7 +52167,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1413" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1413" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1413" t="s">
         <v>50</v>
       </c>
@@ -53138,7 +53158,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="1442" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1442" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1442" t="s">
         <v>50</v>
       </c>
@@ -53587,7 +53607,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="1455" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1455" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1455" t="s">
         <v>51</v>
       </c>
@@ -54451,7 +54471,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1482" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1482" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1482" t="s">
         <v>51</v>
       </c>
@@ -54862,7 +54882,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1494" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1494" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1494" t="s">
         <v>52</v>
       </c>
@@ -55758,7 +55778,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="1522" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1522" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1522" t="s">
         <v>52</v>
       </c>
@@ -55959,7 +55979,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1528" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1528" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1528" t="s">
         <v>53</v>
       </c>
@@ -57047,7 +57067,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1562" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1562" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1562" t="s">
         <v>53</v>
       </c>
@@ -57706,7 +57726,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1581" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1581" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1581" t="s">
         <v>54</v>
       </c>
@@ -57738,7 +57758,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="1582" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1582" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1582" t="s">
         <v>54</v>
       </c>
@@ -58580,7 +58600,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1607" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1607" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1607" t="s">
         <v>55</v>
       </c>
@@ -59772,7 +59792,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1642" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1642" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1642" t="s">
         <v>55</v>
       </c>
@@ -60081,7 +60101,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1651" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1651" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1651" t="s">
         <v>56</v>
       </c>
@@ -61136,7 +61156,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1682" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1682" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1682" t="s">
         <v>56</v>
       </c>
@@ -61620,7 +61640,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1696" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1696" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1696" t="s">
         <v>57</v>
       </c>
@@ -62494,7 +62514,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1722" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1722" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1722" t="s">
         <v>57</v>
       </c>
@@ -62835,7 +62855,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1732" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1732" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1732" t="s">
         <v>58</v>
       </c>
@@ -63795,7 +63815,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1762" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1762" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1762" t="s">
         <v>58</v>
       </c>
@@ -63999,7 +64019,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1768" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1768" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1768" t="s">
         <v>59</v>
       </c>
@@ -65014,7 +65034,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1797" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1797" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1797" t="s">
         <v>59</v>
       </c>
@@ -65795,7 +65815,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1820" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1820" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1820" t="s">
         <v>60</v>
       </c>
@@ -66608,7 +66628,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1844" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1844" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1844" t="s">
         <v>60</v>
       </c>
@@ -66882,7 +66902,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1852" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1852" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1852" t="s">
         <v>61</v>
       </c>
@@ -67969,7 +67989,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1884" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1884" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1884" t="s">
         <v>61</v>
       </c>
@@ -68380,7 +68400,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1896" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1896" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1896" t="s">
         <v>62</v>
       </c>
@@ -69276,7 +69296,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="1924" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1924" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1924" t="s">
         <v>62</v>
       </c>
@@ -69480,7 +69500,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1930" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1930" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1930" t="s">
         <v>63</v>
       </c>
@@ -70640,7 +70660,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1964" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1964" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1964" t="s">
         <v>63</v>
       </c>
@@ -70914,7 +70934,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1972" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1972" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1972" t="s">
         <v>64</v>
       </c>
@@ -72001,7 +72021,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2004" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2004" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2004" t="s">
         <v>64</v>
       </c>
@@ -72415,7 +72435,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2016" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2016" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2016" t="s">
         <v>65</v>
       </c>
@@ -72479,7 +72499,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2018" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2018" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2018" t="s">
         <v>65</v>
       </c>
@@ -74253,7 +74273,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2071" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2071" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2071" t="s">
         <v>66</v>
       </c>
@@ -74672,7 +74692,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2084" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2084" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2084" t="s">
         <v>66</v>
       </c>
@@ -74911,7 +74931,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2091" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2091" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2091" t="s">
         <v>67</v>
       </c>
@@ -76033,7 +76053,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2124" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2124" t="s">
         <v>67</v>
       </c>
@@ -76097,7 +76117,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2126" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2126" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2126" t="s">
         <v>68</v>
       </c>
@@ -77391,7 +77411,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2164" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2164" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2164" t="s">
         <v>68</v>
       </c>
@@ -78120,7 +78140,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2185" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2185" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2185" t="s">
         <v>69</v>
       </c>
@@ -78746,7 +78766,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2204" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2204" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2204" t="s">
         <v>69</v>
       </c>
@@ -79300,7 +79320,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2220" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2220" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2220" t="s">
         <v>70</v>
       </c>
@@ -80104,7 +80124,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2244" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2244" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2244" t="s">
         <v>70</v>
       </c>
@@ -80203,7 +80223,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2247" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2247" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2247" t="s">
         <v>71</v>
       </c>
@@ -81462,7 +81482,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2284" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2284" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2284" t="s">
         <v>71</v>
       </c>
@@ -82331,7 +82351,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2309" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2309" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2309" t="s">
         <v>72</v>
       </c>
@@ -82817,7 +82837,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2324" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2324" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2324" t="s">
         <v>72</v>
       </c>
@@ -83056,7 +83076,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2331" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2331" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2331" t="s">
         <v>73</v>
       </c>
@@ -84175,7 +84195,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2364" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2364" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2364" t="s">
         <v>73</v>
       </c>
@@ -85044,7 +85064,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2389" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2389" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2389" t="s">
         <v>74</v>
       </c>
@@ -85539,7 +85559,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2404" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2404" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2404" t="s">
         <v>74</v>
       </c>
@@ -86268,7 +86288,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="2425" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2425" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2425" t="s">
         <v>75</v>
       </c>
@@ -86888,7 +86908,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2444" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2444" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2444" t="s">
         <v>75</v>
       </c>
@@ -87127,7 +87147,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2451" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2451" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2451" t="s">
         <v>76</v>
       </c>
@@ -88261,7 +88281,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="2484" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2484" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2484" t="s">
         <v>76</v>
       </c>
@@ -88500,7 +88520,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2491" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2491" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2491" t="s">
         <v>77</v>
       </c>
@@ -89631,7 +89651,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2524" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2524" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2524" t="s">
         <v>77</v>
       </c>
@@ -89660,7 +89680,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="2525" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2525" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2525" t="s">
         <v>78</v>
       </c>
@@ -90980,7 +91000,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2564" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2564" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2564" t="s">
         <v>78</v>
       </c>
@@ -91254,7 +91274,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2572" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2572" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2572">
         <v>1709759845287850</v>
       </c>
@@ -92341,7 +92361,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2604" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2604" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2604" t="s">
         <v>79</v>
       </c>
@@ -92580,7 +92600,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2611" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2611" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2611" t="s">
         <v>80</v>
       </c>
@@ -93350,7 +93370,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2633" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2633" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2633" t="s">
         <v>80</v>
       </c>
@@ -94259,7 +94279,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2660" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2660" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2660" t="s">
         <v>81</v>
       </c>
@@ -95054,7 +95074,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2684" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2684" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2684" t="s">
         <v>81</v>
       </c>
@@ -95084,10 +95104,10 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="H1:H2684" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="G1:G2684" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="At what level(s) are BIM-related educational content offered within the identified academic programme?"/>
+        <filter val="1697541525184"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
updating users in production
</commit_message>
<xml_diff>
--- a/frontend/public/assets/files/BIMei Macro Adoption Study.xlsx
+++ b/frontend/public/assets/files/BIMei Macro Adoption Study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MiguelProjects\02. Projects\7)Macro BIM adoption\frontend\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02A4DEB-99AA-468F-BC55-F5AA4EFF4099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB83CC3-F4DE-4A75-BB8D-2F58BD193220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Questionnaire" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Answers" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Answers!$G$1:$G$2684</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Answers!$H$1:$H$2684</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Questionnaire!$C$2:$C$60</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
@@ -3760,7 +3760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCF85EA6-125E-47DB-87D7-2082C385594A}">
   <dimension ref="A2:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -3848,8 +3848,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O2684"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J91" sqref="J91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4029,7 +4029,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -5245,7 +5245,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -5420,7 +5420,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>16</v>
       </c>
@@ -5452,7 +5452,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -7126,7 +7126,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="91" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>17</v>
       </c>
@@ -8146,7 +8146,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>17</v>
       </c>
@@ -8490,7 +8490,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="131" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>18</v>
       </c>
@@ -9400,7 +9400,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>18</v>
       </c>
@@ -9770,7 +9770,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>19</v>
       </c>
@@ -10082,7 +10082,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="177" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>19</v>
       </c>
@@ -11137,7 +11137,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="208" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>20</v>
       </c>
@@ -11977,7 +11977,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="232" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>20</v>
       </c>
@@ -12717,7 +12717,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="254" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>21</v>
       </c>
@@ -13581,7 +13581,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="281" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>21</v>
       </c>
@@ -13995,7 +13995,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="293" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>22</v>
       </c>
@@ -14027,7 +14027,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="294" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>22</v>
       </c>
@@ -15178,7 +15178,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="328" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>23</v>
       </c>
@@ -15808,7 +15808,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="346" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>23</v>
       </c>
@@ -16758,7 +16758,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="374" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>24</v>
       </c>
@@ -17175,7 +17175,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="386" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>24</v>
       </c>
@@ -17906,7 +17906,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="408" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>25</v>
       </c>
@@ -18536,7 +18536,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="426" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>25</v>
       </c>
@@ -19206,7 +19206,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="446" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>26</v>
       </c>
@@ -20256,7 +20256,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="476" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
         <v>26</v>
       </c>
@@ -20518,7 +20518,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="484" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
         <v>27</v>
       </c>
@@ -21774,7 +21774,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="521" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A521" t="s">
         <v>27</v>
       </c>
@@ -21803,7 +21803,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="522" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A522" t="s">
         <v>28</v>
       </c>
@@ -22080,7 +22080,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="530" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
         <v>28</v>
       </c>
@@ -24025,7 +24025,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="586" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="586" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A586" t="s">
         <v>29</v>
       </c>
@@ -24523,7 +24523,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="601" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="601" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A601" t="s">
         <v>29</v>
       </c>
@@ -24762,7 +24762,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="608" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="608" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A608" t="s">
         <v>30</v>
       </c>
@@ -25004,7 +25004,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="615" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="615" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A615" t="s">
         <v>30</v>
       </c>
@@ -26809,7 +26809,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="667" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="667" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A667" t="s">
         <v>31</v>
       </c>
@@ -27266,7 +27266,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="681" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="681" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A681" t="s">
         <v>31</v>
       </c>
@@ -27855,7 +27855,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="698" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="698" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A698" t="s">
         <v>32</v>
       </c>
@@ -28627,7 +28627,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="721" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="721" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A721" t="s">
         <v>32</v>
       </c>
@@ -28866,7 +28866,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="728" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="728" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A728" t="s">
         <v>33</v>
       </c>
@@ -29566,7 +29566,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="748" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="748" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A748" t="s">
         <v>33</v>
       </c>
@@ -30504,7 +30504,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="776" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="776" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A776" t="s">
         <v>34</v>
       </c>
@@ -30924,7 +30924,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="788" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="788" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A788" t="s">
         <v>34</v>
       </c>
@@ -31909,7 +31909,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="817" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="817" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A817" t="s">
         <v>35</v>
       </c>
@@ -32704,7 +32704,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="841" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="841" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A841" t="s">
         <v>35</v>
       </c>
@@ -32733,7 +32733,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="842" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="842" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A842" t="s">
         <v>36</v>
       </c>
@@ -33045,7 +33045,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="851" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="851" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A851" t="s">
         <v>36</v>
       </c>
@@ -34438,7 +34438,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="892" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="892" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A892" t="s">
         <v>37</v>
       </c>
@@ -35366,7 +35366,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="921" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="921" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A921" t="s">
         <v>37</v>
       </c>
@@ -35395,7 +35395,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="922" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="922" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A922" t="s">
         <v>38</v>
       </c>
@@ -35917,7 +35917,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="937" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="937" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A937" t="s">
         <v>38</v>
       </c>
@@ -37016,7 +37016,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="969" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="969" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A969" t="s">
         <v>39</v>
       </c>
@@ -38109,7 +38109,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1001" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1001" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1001" t="s">
         <v>39</v>
       </c>
@@ -38313,7 +38313,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1007" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1007" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1007" t="s">
         <v>40</v>
       </c>
@@ -39479,7 +39479,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="1041" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1041" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1041" t="s">
         <v>40</v>
       </c>
@@ -39823,7 +39823,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="1051" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1051" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1051" t="s">
         <v>41</v>
       </c>
@@ -40783,7 +40783,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1081" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1081" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1081" t="s">
         <v>41</v>
       </c>
@@ -41057,7 +41057,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="1089" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1089" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1089" t="s">
         <v>42</v>
       </c>
@@ -41337,7 +41337,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="1097" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1097" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1097" t="s">
         <v>42</v>
       </c>
@@ -42223,7 +42223,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="1123" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1123" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1123" t="s">
         <v>43</v>
       </c>
@@ -42465,7 +42465,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="1130" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1130" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1130" t="s">
         <v>43</v>
       </c>
@@ -44287,7 +44287,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1183" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1183" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1183" t="s">
         <v>44</v>
       </c>
@@ -44884,7 +44884,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1201" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1201" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1201" t="s">
         <v>44</v>
       </c>
@@ -45018,7 +45018,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1205" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1205" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1205" t="s">
         <v>45</v>
       </c>
@@ -46248,7 +46248,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1241" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1241" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1241" t="s">
         <v>45</v>
       </c>
@@ -46695,7 +46695,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="1253" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1253" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1253" t="s">
         <v>46</v>
       </c>
@@ -47744,7 +47744,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="1281" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1281" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1281" t="s">
         <v>46</v>
       </c>
@@ -48336,7 +48336,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1298" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1298" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1298" t="s">
         <v>47</v>
       </c>
@@ -49096,7 +49096,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1321" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1321" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1321" t="s">
         <v>47</v>
       </c>
@@ -49195,7 +49195,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1324" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1324" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1324" t="s">
         <v>48</v>
       </c>
@@ -50460,7 +50460,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1361" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1361" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1361" t="s">
         <v>48</v>
       </c>
@@ -50979,7 +50979,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="1376" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1376" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1376" t="s">
         <v>49</v>
       </c>
@@ -51779,7 +51779,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1401" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1401" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1401" t="s">
         <v>49</v>
       </c>
@@ -51983,7 +51983,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1407" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1407" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1407" t="s">
         <v>50</v>
       </c>
@@ -52193,7 +52193,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1413" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1413" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1413" t="s">
         <v>50</v>
       </c>
@@ -53184,7 +53184,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="1442" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1442" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1442" t="s">
         <v>50</v>
       </c>
@@ -53633,7 +53633,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="1455" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1455" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1455" t="s">
         <v>51</v>
       </c>
@@ -54497,7 +54497,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1482" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1482" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1482" t="s">
         <v>51</v>
       </c>
@@ -54908,7 +54908,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1494" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1494" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1494" t="s">
         <v>52</v>
       </c>
@@ -55804,7 +55804,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="1522" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1522" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1522" t="s">
         <v>52</v>
       </c>
@@ -56005,7 +56005,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1528" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1528" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1528" t="s">
         <v>53</v>
       </c>
@@ -57093,7 +57093,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1562" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1562" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1562" t="s">
         <v>53</v>
       </c>
@@ -57752,7 +57752,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1581" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1581" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1581" t="s">
         <v>54</v>
       </c>
@@ -57784,7 +57784,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="1582" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1582" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1582" t="s">
         <v>54</v>
       </c>
@@ -58626,7 +58626,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1607" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1607" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1607" t="s">
         <v>55</v>
       </c>
@@ -59818,7 +59818,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1642" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1642" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1642" t="s">
         <v>55</v>
       </c>
@@ -60127,7 +60127,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1651" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1651" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1651" t="s">
         <v>56</v>
       </c>
@@ -61182,7 +61182,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1682" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1682" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1682" t="s">
         <v>56</v>
       </c>
@@ -61666,7 +61666,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1696" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1696" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1696" t="s">
         <v>57</v>
       </c>
@@ -62540,7 +62540,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1722" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1722" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1722" t="s">
         <v>57</v>
       </c>
@@ -62881,7 +62881,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1732" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1732" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1732" t="s">
         <v>58</v>
       </c>
@@ -63841,7 +63841,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1762" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1762" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1762" t="s">
         <v>58</v>
       </c>
@@ -64045,7 +64045,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1768" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1768" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1768" t="s">
         <v>59</v>
       </c>
@@ -65060,7 +65060,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1797" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1797" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1797" t="s">
         <v>59</v>
       </c>
@@ -65841,7 +65841,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1820" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1820" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1820" t="s">
         <v>60</v>
       </c>
@@ -66654,7 +66654,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1844" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1844" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1844" t="s">
         <v>60</v>
       </c>
@@ -66928,7 +66928,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1852" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1852" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1852" t="s">
         <v>61</v>
       </c>
@@ -68015,7 +68015,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1884" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1884" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1884" t="s">
         <v>61</v>
       </c>
@@ -68426,7 +68426,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1896" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1896" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1896" t="s">
         <v>62</v>
       </c>
@@ -69322,7 +69322,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="1924" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1924" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1924" t="s">
         <v>62</v>
       </c>
@@ -69526,7 +69526,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1930" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1930" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1930" t="s">
         <v>63</v>
       </c>
@@ -70686,7 +70686,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1964" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1964" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1964" t="s">
         <v>63</v>
       </c>
@@ -70960,7 +70960,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="1972" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1972" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1972" t="s">
         <v>64</v>
       </c>
@@ -72047,7 +72047,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2004" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2004" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2004" t="s">
         <v>64</v>
       </c>
@@ -72461,7 +72461,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2016" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2016" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2016" t="s">
         <v>65</v>
       </c>
@@ -72525,7 +72525,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2018" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2018" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2018" t="s">
         <v>65</v>
       </c>
@@ -74299,7 +74299,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2071" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2071" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2071" t="s">
         <v>66</v>
       </c>
@@ -74718,7 +74718,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2084" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2084" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2084" t="s">
         <v>66</v>
       </c>
@@ -74957,7 +74957,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2091" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2091" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2091" t="s">
         <v>67</v>
       </c>
@@ -76079,7 +76079,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2124" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2124" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2124" t="s">
         <v>67</v>
       </c>
@@ -76143,7 +76143,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2126" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2126" t="s">
         <v>68</v>
       </c>
@@ -77437,7 +77437,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2164" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2164" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2164" t="s">
         <v>68</v>
       </c>
@@ -78166,7 +78166,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2185" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2185" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2185" t="s">
         <v>69</v>
       </c>
@@ -78792,7 +78792,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2204" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2204" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2204" t="s">
         <v>69</v>
       </c>
@@ -79346,7 +79346,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2220" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2220" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2220" t="s">
         <v>70</v>
       </c>
@@ -80150,7 +80150,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2244" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2244" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2244" t="s">
         <v>70</v>
       </c>
@@ -80249,7 +80249,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2247" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2247" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2247" t="s">
         <v>71</v>
       </c>
@@ -81508,7 +81508,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2284" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2284" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2284" t="s">
         <v>71</v>
       </c>
@@ -82377,7 +82377,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2309" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2309" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2309" t="s">
         <v>72</v>
       </c>
@@ -82863,7 +82863,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2324" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2324" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2324" t="s">
         <v>72</v>
       </c>
@@ -83102,7 +83102,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2331" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2331" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2331" t="s">
         <v>73</v>
       </c>
@@ -84221,7 +84221,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2364" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2364" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2364" t="s">
         <v>73</v>
       </c>
@@ -85090,7 +85090,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2389" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2389" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2389" t="s">
         <v>74</v>
       </c>
@@ -85585,7 +85585,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2404" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2404" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2404" t="s">
         <v>74</v>
       </c>
@@ -86314,7 +86314,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="2425" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2425" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2425" t="s">
         <v>75</v>
       </c>
@@ -86934,7 +86934,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2444" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2444" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2444" t="s">
         <v>75</v>
       </c>
@@ -87173,7 +87173,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2451" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2451" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2451" t="s">
         <v>76</v>
       </c>
@@ -88307,7 +88307,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="2484" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2484" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2484" t="s">
         <v>76</v>
       </c>
@@ -88546,7 +88546,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2491" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2491" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2491" t="s">
         <v>77</v>
       </c>
@@ -89677,7 +89677,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2524" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2524" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2524" t="s">
         <v>77</v>
       </c>
@@ -89706,7 +89706,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="2525" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2525" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2525" t="s">
         <v>78</v>
       </c>
@@ -91026,7 +91026,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2564" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2564" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2564" t="s">
         <v>78</v>
       </c>
@@ -91300,7 +91300,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2572" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2572" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2572">
         <v>1709759845287850</v>
       </c>
@@ -92387,7 +92387,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2604" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2604" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2604" t="s">
         <v>79</v>
       </c>
@@ -92626,7 +92626,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2611" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2611" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2611" t="s">
         <v>80</v>
       </c>
@@ -93396,7 +93396,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2633" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2633" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2633" t="s">
         <v>80</v>
       </c>
@@ -94305,7 +94305,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2660" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2660" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2660" t="s">
         <v>81</v>
       </c>
@@ -95100,7 +95100,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="2684" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2684" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2684" t="s">
         <v>81</v>
       </c>
@@ -95130,10 +95130,10 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="G1:G2684" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="H1:H2684" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="1697541525184"/>
+        <filter val="At what level(s) are BIM-related educational content offered within the identified academic programme?"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>